<commit_message>
added lots of stuff
</commit_message>
<xml_diff>
--- a/Data Files/processes.xlsx
+++ b/Data Files/processes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.donose\git\GAS_AUTOMATION\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E0A097-9CE8-4382-BF86-27678F170531}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37965D60-43D4-4C6F-85F0-E200CD5B7247}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5940" yWindow="3030" windowWidth="21600" windowHeight="11385" xr2:uid="{EFDD7002-98FF-4161-9AEB-61B3F947A031}"/>
+    <workbookView xWindow="-28020" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{EFDD7002-98FF-4161-9AEB-61B3F947A031}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
     <t>Offer</t>
   </si>
   <si>
-    <t>ME-405</t>
+    <t>ME-427</t>
   </si>
 </sst>
 </file>
@@ -437,7 +437,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
need to edit CT  objectx xpath
</commit_message>
<xml_diff>
--- a/Data Files/processes.xlsx
+++ b/Data Files/processes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.donose\git\GAS_AUTOMATION\Data Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.donose\git\GAS_V4\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7015F02-978A-4033-8AE6-268EFD556DA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E7674A-B6C9-411A-A981-1F34486A317E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28020" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{EFDD7002-98FF-4161-9AEB-61B3F947A031}"/>
   </bookViews>
@@ -41,10 +41,10 @@
     <t>Contract</t>
   </si>
   <si>
-    <t>ME-491</t>
+    <t>ME-510</t>
   </si>
   <si>
-    <t xml:space="preserve">CT-255 </t>
+    <t>CT-249</t>
   </si>
 </sst>
 </file>
@@ -452,7 +452,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
function to check text/ no need for all objects
</commit_message>
<xml_diff>
--- a/Data Files/processes.xlsx
+++ b/Data Files/processes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.donose\git\GAS_V4\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7BFCC3-3C6D-4007-9FF6-182A59411271}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0BEBB7-3E5C-4E42-8623-F2E87881008C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24075" yWindow="990" windowWidth="21600" windowHeight="11385" xr2:uid="{EFDD7002-98FF-4161-9AEB-61B3F947A031}"/>
+    <workbookView xWindow="-20010" yWindow="1110" windowWidth="21600" windowHeight="11385" xr2:uid="{EFDD7002-98FF-4161-9AEB-61B3F947A031}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>Meeting</t>
   </si>
@@ -41,19 +41,46 @@
     <t>Contract</t>
   </si>
   <si>
-    <t>ME-516</t>
-  </si>
-  <si>
-    <t>CT-244</t>
-  </si>
-  <si>
     <t>Billing req</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t xml:space="preserve">rom 0 </t>
+    <t>CT-274</t>
+  </si>
+  <si>
+    <t>OF-551</t>
+  </si>
+  <si>
+    <t>ME-553</t>
+  </si>
+  <si>
+    <t>ME-554</t>
+  </si>
+  <si>
+    <t>ME-555</t>
+  </si>
+  <si>
+    <t>ME-556</t>
+  </si>
+  <si>
+    <t>ME-557</t>
+  </si>
+  <si>
+    <t>ME-558</t>
+  </si>
+  <si>
+    <t>ME-559</t>
+  </si>
+  <si>
+    <t>OF-564</t>
+  </si>
+  <si>
+    <t>ME-560</t>
+  </si>
+  <si>
+    <t>OF-565</t>
   </si>
 </sst>
 </file>
@@ -471,14 +498,14 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="8.85546875" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -492,17 +519,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="1"/>

</xml_diff>

<commit_message>
added fromMeeting and fromOffer text chekers
</commit_message>
<xml_diff>
--- a/Data Files/processes.xlsx
+++ b/Data Files/processes.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>Meeting</t>
   </si>
@@ -81,6 +81,15 @@
   </si>
   <si>
     <t>OF-565</t>
+  </si>
+  <si>
+    <t>ME-561</t>
+  </si>
+  <si>
+    <t>ME-562</t>
+  </si>
+  <si>
+    <t>OF-567</t>
   </si>
 </sst>
 </file>
@@ -526,10 +535,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
massive update! new link process system
</commit_message>
<xml_diff>
--- a/Data Files/processes.xlsx
+++ b/Data Files/processes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.donose\git\GAS_V4\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0BEBB7-3E5C-4E42-8623-F2E87881008C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F061518D-72D0-45F4-882D-412D46061373}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20010" yWindow="1110" windowWidth="21600" windowHeight="11385" xr2:uid="{EFDD7002-98FF-4161-9AEB-61B3F947A031}"/>
+    <workbookView xWindow="-23850" yWindow="2310" windowWidth="21600" windowHeight="11385" xr2:uid="{EFDD7002-98FF-4161-9AEB-61B3F947A031}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Meeting</t>
   </si>
@@ -44,52 +44,52 @@
     <t>Billing req</t>
   </si>
   <si>
+    <t>Billing inv</t>
+  </si>
+  <si>
+    <t>ME-632</t>
+  </si>
+  <si>
+    <t>OF-637</t>
+  </si>
+  <si>
+    <t>CT-304</t>
+  </si>
+  <si>
+    <t>BR-414</t>
+  </si>
+  <si>
+    <t>BI-139</t>
+  </si>
+  <si>
+    <t>Receivables</t>
+  </si>
+  <si>
+    <t>RE-69</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>CT-274</t>
-  </si>
-  <si>
-    <t>OF-551</t>
-  </si>
-  <si>
-    <t>ME-553</t>
-  </si>
-  <si>
-    <t>ME-554</t>
-  </si>
-  <si>
-    <t>ME-555</t>
-  </si>
-  <si>
-    <t>ME-556</t>
-  </si>
-  <si>
-    <t>ME-557</t>
-  </si>
-  <si>
-    <t>ME-558</t>
-  </si>
-  <si>
-    <t>ME-559</t>
-  </si>
-  <si>
-    <t>OF-564</t>
-  </si>
-  <si>
-    <t>ME-560</t>
-  </si>
-  <si>
-    <t>OF-565</t>
-  </si>
-  <si>
-    <t>ME-561</t>
-  </si>
-  <si>
-    <t>ME-562</t>
-  </si>
-  <si>
-    <t>OF-567</t>
+    <t>ME-633</t>
+  </si>
+  <si>
+    <t>OF-638</t>
+  </si>
+  <si>
+    <t>CT-305</t>
+  </si>
+  <si>
+    <t>BR-419</t>
+  </si>
+  <si>
+    <t>BI-143</t>
+  </si>
+  <si>
+    <t>ME-634</t>
+  </si>
+  <si>
+    <t>OF-639</t>
   </si>
 </sst>
 </file>
@@ -114,7 +114,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,6 +142,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -173,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -188,6 +194,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -507,7 +516,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,6 +524,8 @@
     <col min="1" max="1" customWidth="true" width="8.85546875" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="23.7109375" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -530,8 +541,12 @@
       <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -541,13 +556,17 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>

</xml_diff>

<commit_message>
to make scroll to position
</commit_message>
<xml_diff>
--- a/Data Files/processes.xlsx
+++ b/Data Files/processes.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.donose\git\GAS_V4\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F061518D-72D0-45F4-882D-412D46061373}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F39486C-8988-4493-A6E4-F9CD2489E0DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23850" yWindow="2310" windowWidth="21600" windowHeight="11385" xr2:uid="{EFDD7002-98FF-4161-9AEB-61B3F947A031}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Meeting</t>
   </si>
@@ -47,57 +47,44 @@
     <t>Billing inv</t>
   </si>
   <si>
-    <t>ME-632</t>
-  </si>
-  <si>
-    <t>OF-637</t>
-  </si>
-  <si>
-    <t>CT-304</t>
-  </si>
-  <si>
-    <t>BR-414</t>
-  </si>
-  <si>
-    <t>BI-139</t>
-  </si>
-  <si>
     <t>Receivables</t>
   </si>
   <si>
-    <t>RE-69</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>ME-633</t>
-  </si>
-  <si>
-    <t>OF-638</t>
-  </si>
-  <si>
-    <t>CT-305</t>
-  </si>
-  <si>
-    <t>BR-419</t>
-  </si>
-  <si>
-    <t>BI-143</t>
-  </si>
-  <si>
-    <t>ME-634</t>
-  </si>
-  <si>
-    <t>OF-639</t>
+    <t>ME-638</t>
+  </si>
+  <si>
+    <t>OF-643</t>
+  </si>
+  <si>
+    <t>CT-308</t>
+  </si>
+  <si>
+    <t>BR-434</t>
+  </si>
+  <si>
+    <t>BI-146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RE-76 </t>
+  </si>
+  <si>
+    <t>Sale Order</t>
+  </si>
+  <si>
+    <t>OR-207</t>
+  </si>
+  <si>
+    <t>Purchase req</t>
+  </si>
+  <si>
+    <t>POR-897</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,7 +101,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,6 +135,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -179,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -197,6 +196,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -513,22 +518,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{802F6526-6E56-49DE-B99E-BCFDB4DEA65E}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="1" max="1" width="8.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -545,30 +552,42 @@
         <v>4</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -576,7 +595,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>

</xml_diff>

<commit_message>
now linkers are from SQL
</commit_message>
<xml_diff>
--- a/Data Files/processes.xlsx
+++ b/Data Files/processes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.donose\git\GAS_V4\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C34A07C-0F91-4A78-9E0B-55B2635EC347}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38359AE4-00B1-414B-B257-B9A2C2517FE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25680" yWindow="3630" windowWidth="21600" windowHeight="11385" xr2:uid="{EFDD7002-98FF-4161-9AEB-61B3F947A031}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
   <si>
     <t>Meeting</t>
   </si>
@@ -59,244 +59,70 @@
     <t>Purchase order</t>
   </si>
   <si>
-    <t>BR-541</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
-    <t>BI-203</t>
-  </si>
-  <si>
-    <t>ME-721</t>
-  </si>
-  <si>
-    <t>OF-726</t>
-  </si>
-  <si>
-    <t>ME-722</t>
-  </si>
-  <si>
-    <t>OF-727</t>
-  </si>
-  <si>
-    <t>CT-363</t>
-  </si>
-  <si>
-    <t>OR-249</t>
-  </si>
-  <si>
-    <t>ME-723</t>
-  </si>
-  <si>
-    <t>ME-724</t>
-  </si>
-  <si>
-    <t>OF-729</t>
-  </si>
-  <si>
-    <t>CT-364</t>
-  </si>
-  <si>
-    <t>OR-250</t>
-  </si>
-  <si>
-    <t>ME-725</t>
-  </si>
-  <si>
-    <t>ME-726</t>
-  </si>
-  <si>
-    <t>OF-731</t>
-  </si>
-  <si>
-    <t>CT-365</t>
-  </si>
-  <si>
-    <t>OR-251</t>
-  </si>
-  <si>
-    <t>ME-727</t>
-  </si>
-  <si>
-    <t>OF-732</t>
-  </si>
-  <si>
-    <t>CT-366</t>
-  </si>
-  <si>
-    <t>OR-252</t>
-  </si>
-  <si>
-    <t>ME-728</t>
-  </si>
-  <si>
-    <t>OF-733</t>
-  </si>
-  <si>
-    <t>CT-367</t>
-  </si>
-  <si>
-    <t>OR-253</t>
-  </si>
-  <si>
-    <t>ME-729</t>
-  </si>
-  <si>
-    <t>OF-734</t>
-  </si>
-  <si>
-    <t>CT-368</t>
-  </si>
-  <si>
-    <t>ME-730</t>
-  </si>
-  <si>
-    <t>OF-735</t>
-  </si>
-  <si>
-    <t>ME-731</t>
-  </si>
-  <si>
-    <t>ME-732</t>
-  </si>
-  <si>
-    <t>ME-733</t>
-  </si>
-  <si>
-    <t>OF-738</t>
-  </si>
-  <si>
-    <t>CT-369</t>
-  </si>
-  <si>
-    <t>BR-545</t>
-  </si>
-  <si>
-    <t>BI-204</t>
-  </si>
-  <si>
-    <t>ME-734</t>
-  </si>
-  <si>
-    <t>ME-735</t>
-  </si>
-  <si>
-    <t>OF-740</t>
-  </si>
-  <si>
-    <t>CT-370</t>
-  </si>
-  <si>
-    <t>BR-546</t>
-  </si>
-  <si>
-    <t>BI-205</t>
-  </si>
-  <si>
-    <t>ME-736</t>
-  </si>
-  <si>
-    <t>OF-741</t>
-  </si>
-  <si>
-    <t>CT-371</t>
-  </si>
-  <si>
-    <t>BR-547</t>
-  </si>
-  <si>
-    <t>BI-206</t>
-  </si>
-  <si>
-    <t>ME-737</t>
-  </si>
-  <si>
-    <t>ME-738</t>
-  </si>
-  <si>
-    <t>OF-743</t>
-  </si>
-  <si>
-    <t>CT-372</t>
-  </si>
-  <si>
-    <t>BR-548</t>
-  </si>
-  <si>
-    <t>BI-207</t>
-  </si>
-  <si>
-    <t>ME-739</t>
-  </si>
-  <si>
-    <t>OF-744</t>
-  </si>
-  <si>
-    <t>ME-740</t>
-  </si>
-  <si>
-    <t>OF-745</t>
-  </si>
-  <si>
-    <t>CT-373</t>
-  </si>
-  <si>
-    <t>BR-549</t>
-  </si>
-  <si>
-    <t>BI-208</t>
-  </si>
-  <si>
-    <t>RE-132</t>
-  </si>
-  <si>
-    <t>ME-741</t>
-  </si>
-  <si>
-    <t>ME-742</t>
-  </si>
-  <si>
-    <t>ME-743</t>
-  </si>
-  <si>
-    <t>OF-748</t>
-  </si>
-  <si>
-    <t>CT-374</t>
-  </si>
-  <si>
-    <t>BR-550</t>
-  </si>
-  <si>
-    <t>BI-209</t>
-  </si>
-  <si>
-    <t>ME-744</t>
-  </si>
-  <si>
-    <t>ME-745</t>
-  </si>
-  <si>
-    <t>ME-746</t>
-  </si>
-  <si>
-    <t>ME-747</t>
-  </si>
-  <si>
-    <t>ME-748</t>
-  </si>
-  <si>
-    <t>ME-749</t>
-  </si>
-  <si>
-    <t>ME-750</t>
-  </si>
-  <si>
-    <t>OF-753</t>
-  </si>
-  <si>
-    <t>CT-375</t>
+    <t>ME-768</t>
+  </si>
+  <si>
+    <t>OF-773</t>
+  </si>
+  <si>
+    <t>CT-390</t>
+  </si>
+  <si>
+    <t>BR-572</t>
+  </si>
+  <si>
+    <t>BI-223</t>
+  </si>
+  <si>
+    <t>RE-147</t>
+  </si>
+  <si>
+    <t>OR-269</t>
+  </si>
+  <si>
+    <t>ME-769</t>
+  </si>
+  <si>
+    <t>OF-774</t>
+  </si>
+  <si>
+    <t>ME-770</t>
+  </si>
+  <si>
+    <t>ME-772</t>
+  </si>
+  <si>
+    <t>ME-773</t>
+  </si>
+  <si>
+    <t>ME-774</t>
+  </si>
+  <si>
+    <t>pened.</t>
+  </si>
+  <si>
+    <t>ME-777</t>
+  </si>
+  <si>
+    <t>ME-778</t>
+  </si>
+  <si>
+    <t>OF-783</t>
+  </si>
+  <si>
+    <t>CT-391</t>
+  </si>
+  <si>
+    <t>BR-573</t>
+  </si>
+  <si>
+    <t>Please</t>
+  </si>
+  <si>
+    <t>OR-275</t>
   </si>
 </sst>
 </file>
@@ -750,7 +576,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,22 +622,28 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>72</v>
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>